<commit_message>
add risk management plan file
</commit_message>
<xml_diff>
--- a/document/risk_management_plan.xlsx
+++ b/document/risk_management_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kesiah Dupo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-hypertechs-2-0\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Moderate</t>
-  </si>
-  <si>
-    <t>SCRIBE</t>
   </si>
   <si>
     <t>Hypertechs-2.0</t>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>Project Name:</t>
+  </si>
+  <si>
+    <t>SCRIBE APP</t>
   </si>
 </sst>
 </file>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -733,19 +733,19 @@
     <col min="7" max="7" width="23.796875" style="11" customWidth="1"/>
     <col min="8" max="8" width="22.3984375" style="11" customWidth="1"/>
     <col min="9" max="9" width="14.59765625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="14" customWidth="1"/>
+    <col min="10" max="10" width="13.69921875" style="14" customWidth="1"/>
     <col min="11" max="12" width="8.59765625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="21.296875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="22.59765625" style="11" customWidth="1"/>
     <col min="14" max="25" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="22" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -760,11 +760,11 @@
     </row>
     <row r="2" spans="1:13" ht="16.8" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -779,7 +779,7 @@
     </row>
     <row r="3" spans="1:13" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="3"/>
@@ -843,16 +843,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>16</v>
@@ -861,7 +861,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>19</v>
@@ -873,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="58.2" customHeight="1">
@@ -902,7 +902,7 @@
         <v>26</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>27</v>
@@ -943,7 +943,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>27</v>
@@ -963,28 +963,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="I8" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>27</v>
@@ -996,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="46.8" customHeight="1">
@@ -1025,7 +1025,7 @@
         <v>41</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>27</v>
@@ -1066,7 +1066,7 @@
         <v>48</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>27</v>
@@ -1101,13 +1101,13 @@
         <v>53</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>54</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>27</v>
@@ -1148,7 +1148,7 @@
         <v>61</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>18</v>

</xml_diff>